<commit_message>
Main. Functions done. Exe added. Documentation added
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -601,12 +601,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>55</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>53</t>
         </is>
       </c>
       <c r="K3" t="n">
@@ -663,12 +663,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>15</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>14</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -725,12 +725,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
           <t>7</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>6</t>
         </is>
       </c>
       <c r="K5" t="n">
@@ -787,12 +787,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>115</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>115</t>
+          <t>120</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -849,12 +849,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
           <t>31</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>30</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -911,12 +911,12 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>58</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>60</t>
         </is>
       </c>
       <c r="K8" t="n">

</xml_diff>